<commit_message>
Mise à jour des bases avant diffusion
</commit_message>
<xml_diff>
--- a/Remote/ug16/Données/03/dist_coûts.xlsx
+++ b/Remote/ug16/Données/03/dist_coûts.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Mickaël\Documents\GitHub\ductaironline\Remote\ug16\Données\04\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84DCBF28-6C9E-4F0C-A645-10481F46A76E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFEA8A83-B7E6-4D36-AFB0-90EFB478AE49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="78">
   <si>
     <t>id</t>
   </si>
@@ -267,6 +267,9 @@
   </si>
   <si>
     <t>Mo_Spé</t>
+  </si>
+  <si>
+    <t>Spécifique</t>
   </si>
 </sst>
 </file>
@@ -725,10 +728,10 @@
         <v>68</v>
       </c>
       <c r="Z1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AA1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
@@ -802,13 +805,13 @@
         <v>45</v>
       </c>
       <c r="Y2">
-        <v>67</v>
+        <v>2.25</v>
       </c>
       <c r="Z2">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="AA2">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
@@ -882,13 +885,13 @@
         <v>40</v>
       </c>
       <c r="Y3">
-        <v>68</v>
+        <v>2.25</v>
       </c>
       <c r="Z3">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="AA3">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
@@ -962,13 +965,13 @@
         <v>35</v>
       </c>
       <c r="Y4">
-        <v>69</v>
+        <v>2.25</v>
       </c>
       <c r="Z4">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="AA4">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
@@ -1042,13 +1045,13 @@
         <v>30</v>
       </c>
       <c r="Y5">
-        <v>70</v>
+        <v>2.25</v>
       </c>
       <c r="Z5">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="AA5">
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
@@ -1113,13 +1116,13 @@
         <v>25</v>
       </c>
       <c r="Y6">
-        <v>71</v>
+        <v>2.25</v>
       </c>
       <c r="Z6">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="AA6">
-        <v>14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
@@ -1424,6 +1427,18 @@
       </c>
       <c r="U11" s="2">
         <v>45748</v>
+      </c>
+      <c r="W11" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y11">
+        <v>1</v>
+      </c>
+      <c r="Z11">
+        <v>0</v>
+      </c>
+      <c r="AA11">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">

</xml_diff>